<commit_message>
* Add 2020 MSC platform history and related excel data. * Add Resume time as criteria. * Add WoV pass criteria. * Add Fan and dGPU section.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FAE32D-13CC-464B-8721-7A0886751CAD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8181A2F2-A390-4CF2-85EE-4E104F4170CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{C78077D0-701F-4057-A844-DDE1B4D08E6E}"/>
   </bookViews>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="85">
   <si>
     <t>Year</t>
   </si>
@@ -104,9 +103,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Y, disable default</t>
   </si>
   <si>
     <t>Y</t>
@@ -288,6 +284,9 @@
   </si>
   <si>
     <t>Oreti MSC</t>
+  </si>
+  <si>
+    <t>Y.  Disable default</t>
   </si>
 </sst>
 </file>
@@ -925,6 +924,7 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -934,34 +934,33 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1276,1373 +1275,1699 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C227EB0F-B6DB-4CE9-BC6C-A64C8559E7C2}">
-  <dimension ref="E10:W51"/>
+  <dimension ref="E10:W68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47:P49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57:H68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" customWidth="1"/>
     <col min="22" max="22" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E11" s="47" t="s">
+    <row r="10" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="G11" s="52"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="54" t="s">
+      <c r="J11" s="55"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="53"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="57" t="s">
+      <c r="M11" s="58"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="56"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="57" t="s">
+      <c r="P11" s="58"/>
+      <c r="Q11" s="59"/>
+    </row>
+    <row r="12" spans="5:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="E12" s="49"/>
+      <c r="F12" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="58"/>
-    </row>
-    <row r="12" spans="5:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E12" s="48"/>
-      <c r="F12" s="39" t="s">
+      <c r="G12" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="H12" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>61</v>
-      </c>
       <c r="I12" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="K12" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="39" t="s">
-        <v>61</v>
-      </c>
       <c r="L12" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="39" t="s">
+      <c r="N12" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N12" s="39" t="s">
-        <v>61</v>
-      </c>
       <c r="O12" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="P12" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="P12" s="39" t="s">
+      <c r="Q12" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="Q12" s="39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="49"/>
+    </row>
+    <row r="13" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="50"/>
       <c r="F13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="O13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="P13" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q13" s="40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="M13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="N13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="O13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="P13" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q13" s="40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E14" s="41" t="s">
-        <v>63</v>
-      </c>
       <c r="F14" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G14" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J14" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K14" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L14" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M14" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N14" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O14" s="42"/>
       <c r="P14" s="42"/>
       <c r="Q14" s="42"/>
     </row>
-    <row r="15" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E15" s="41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J15" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K15" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L15" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M15" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N15" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O15" s="42"/>
       <c r="P15" s="42"/>
       <c r="Q15" s="42"/>
     </row>
-    <row r="16" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E16" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I16" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J16" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K16" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L16" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M16" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N16" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O16" s="42"/>
       <c r="P16" s="42"/>
       <c r="Q16" s="42"/>
     </row>
-    <row r="17" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G17" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J17" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K17" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L17" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M17" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N17" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O17" s="42"/>
       <c r="P17" s="42"/>
       <c r="Q17" s="42"/>
     </row>
-    <row r="18" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I18" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J18" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K18" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L18" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M18" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N18" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O18" s="42"/>
       <c r="P18" s="42"/>
       <c r="Q18" s="42"/>
     </row>
-    <row r="19" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K19" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L19" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M19" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N19" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O19" s="42"/>
       <c r="P19" s="42"/>
       <c r="Q19" s="42"/>
     </row>
-    <row r="20" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I20" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K20" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L20" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M20" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N20" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O20" s="42"/>
       <c r="P20" s="42"/>
       <c r="Q20" s="42"/>
     </row>
-    <row r="21" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J21" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K21" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L21" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M21" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N21" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O21" s="42"/>
       <c r="P21" s="42"/>
       <c r="Q21" s="42"/>
     </row>
-    <row r="22" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E22" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="42" t="s">
+      <c r="H22" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" s="46" t="s">
-        <v>75</v>
-      </c>
       <c r="J22" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K22" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L22" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M22" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N22" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O22" s="46"/>
       <c r="P22" s="46"/>
       <c r="Q22" s="46"/>
     </row>
-    <row r="25" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="47" t="s">
-        <v>54</v>
+    <row r="25" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="48" t="s">
+        <v>53</v>
       </c>
       <c r="F26" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" s="52"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="50"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="54" t="s">
+      <c r="J26" s="55"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="J26" s="53"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="57" t="s">
+      <c r="M26" s="58"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+    </row>
+    <row r="27" spans="5:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="E27" s="49"/>
+      <c r="F27" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="K27" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="L27" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="M27" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="N27" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+    </row>
+    <row r="28" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="50"/>
+      <c r="F28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="I28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="J28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="K28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="M28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="N28" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="47"/>
+    </row>
+    <row r="29" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="N29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="47"/>
+    </row>
+    <row r="30" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="K30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="47"/>
+    </row>
+    <row r="31" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I31" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K31" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="M31" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="N31" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="O31" s="47"/>
+      <c r="P31" s="47"/>
+      <c r="Q31" s="47"/>
+    </row>
+    <row r="32" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K32" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L32" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="N32" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O32" s="47"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="47"/>
+    </row>
+    <row r="33" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="I33" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K33" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L33" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N33" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="O33" s="47"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="47"/>
+    </row>
+    <row r="34" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E34" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="I34" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K34" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M34" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N34" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
+      <c r="Q34" s="47"/>
+    </row>
+    <row r="35" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="I35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="M35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+    </row>
+    <row r="36" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K36" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L36" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M36" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N36" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+    </row>
+    <row r="37" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J37" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K37" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L37" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M37" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N37" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O37" s="47"/>
+      <c r="P37" s="47"/>
+      <c r="Q37" s="47"/>
+    </row>
+    <row r="38" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="5:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E40" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" s="52"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="M26" s="56"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-    </row>
-    <row r="27" spans="5:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E27" s="48"/>
-      <c r="F27" s="39" t="s">
+      <c r="J40" s="55"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="M40" s="58"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="P40" s="52"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="S40" s="55"/>
+      <c r="T40" s="56"/>
+      <c r="U40" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="V40" s="58"/>
+      <c r="W40" s="59"/>
+    </row>
+    <row r="41" spans="5:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="E41" s="49"/>
+      <c r="F41" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="39" t="s">
+      <c r="H41" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="39" t="s">
+      <c r="I41" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="J41" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="39" t="s">
+      <c r="K41" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="K27" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="L27" s="39" t="s">
+      <c r="L41" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="M41" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="M27" s="39" t="s">
+      <c r="N41" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N27" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-    </row>
-    <row r="28" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E28" s="49"/>
-      <c r="F28" s="40" t="s">
+      <c r="O41" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="P41" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q41" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="R41" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="S41" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="T41" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="U41" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="V41" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="W41" s="39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E42" s="50"/>
+      <c r="F42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="I42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="J42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="K42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="L42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="M42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="N42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="O42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="P42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="R42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="S42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="T42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="U42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="V42" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="W42" s="40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E43" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G28" s="40" t="s">
+      <c r="F43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="K43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="N43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="P43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="R43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="T43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="U43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V43" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="W43" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E44" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="K44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="N44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="P44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="R44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="T44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="U44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V44" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="W44" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E45" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J45" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M45" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="P45" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="R45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S45" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="T45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="U45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V45" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="W45" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E46" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M46" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="P46" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="R46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S46" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="T46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="U46" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V46" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="W46" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="I47" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J47" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L47" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M47" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="N47" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="O47" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="P47" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q47" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="R47" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S47" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="T47" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="U47" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V47" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="W47" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G48" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H48" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="I48" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J48" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="K48" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L48" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M48" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="N48" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="O48" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="P48" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q48" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="R48" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S48" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="T48" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="U48" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V48" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="W48" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E49" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="J49" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="K49" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L49" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="M49" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="N49" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="O49" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="P49" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q49" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="R49" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S49" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="T49" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="U49" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V49" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="W49" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E50" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J50" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M50" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="P50" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="R50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S50" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="T50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="U50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V50" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="W50" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E51" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="H51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J51" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="K51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="M51" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="N51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="O51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="P51" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="R51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="S51" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="T51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="U51" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="V51" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="W51" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="5:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E57" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F57" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="G57" s="58"/>
+      <c r="H57" s="59"/>
+    </row>
+    <row r="58" spans="5:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="E58" s="49"/>
+      <c r="F58" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="G58" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="H58" s="39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E59" s="50"/>
+      <c r="F59" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H59" s="40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E60" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="I28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="J28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="K28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="L28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="M28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="N28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-    </row>
-    <row r="29" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E29" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="K29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N29" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
-    </row>
-    <row r="30" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E30" s="41" t="s">
+      <c r="F60" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G60" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H60" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E61" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G61" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H61" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E62" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="K30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N30" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O30" s="59"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="59"/>
-    </row>
-    <row r="31" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E31" s="41" t="s">
+      <c r="F62" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H62" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E63" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="H31" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I31" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J31" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K31" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L31" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="M31" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="N31" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="59"/>
-    </row>
-    <row r="32" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E32" s="41" t="s">
+      <c r="F63" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G63" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H63" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E64" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="H32" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I32" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J32" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K32" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L32" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M32" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N32" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O32" s="59"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
-    </row>
-    <row r="33" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E33" s="44" t="s">
+      <c r="F64" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G64" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H64" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E65" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="F33" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="I33" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J33" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K33" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="L33" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M33" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N33" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="O33" s="59"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="59"/>
-    </row>
-    <row r="34" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E34" s="44" t="s">
+      <c r="F65" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G65" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H65" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E66" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="H34" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="I34" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J34" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K34" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="L34" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M34" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N34" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="O34" s="59"/>
-      <c r="P34" s="59"/>
-      <c r="Q34" s="59"/>
-    </row>
-    <row r="35" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E35" s="44" t="s">
+      <c r="F66" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G66" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H66" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E67" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="F35" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="G35" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="I35" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="J35" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K35" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="L35" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="M35" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N35" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="O35" s="59"/>
-      <c r="P35" s="59"/>
-      <c r="Q35" s="59"/>
-    </row>
-    <row r="36" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E36" s="41" t="s">
+      <c r="F67" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G67" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H67" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E68" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="F36" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="H36" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I36" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J36" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K36" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L36" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M36" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N36" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-    </row>
-    <row r="37" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E37" s="41" t="s">
+      <c r="F68" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G68" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G37" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="H37" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I37" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J37" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K37" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L37" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M37" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N37" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O37" s="59"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="59"/>
-    </row>
-    <row r="38" spans="5:23" x14ac:dyDescent="0.3">
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="5:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E40" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="G40" s="50"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="J40" s="53"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="M40" s="56"/>
-      <c r="N40" s="58"/>
-      <c r="O40" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="S40" s="53"/>
-      <c r="T40" s="55"/>
-      <c r="U40" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="V40" s="56"/>
-      <c r="W40" s="58"/>
-    </row>
-    <row r="41" spans="5:23" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E41" s="48"/>
-      <c r="F41" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="G41" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="H41" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="I41" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="J41" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="K41" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="L41" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="M41" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="N41" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="O41" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="P41" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q41" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="R41" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="S41" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="T41" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="U41" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="V41" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="W41" s="39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E42" s="49"/>
-      <c r="F42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="G42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="H42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="I42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="J42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="K42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="L42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="M42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="N42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="O42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="P42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="R42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="S42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="T42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="U42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="V42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="W42" s="40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="K43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q43" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R43" s="42"/>
-      <c r="S43" s="42"/>
-      <c r="T43" s="42"/>
-      <c r="U43" s="42"/>
-      <c r="V43" s="42"/>
-      <c r="W43" s="42"/>
-    </row>
-    <row r="44" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E44" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="K44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q44" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R44" s="42"/>
-      <c r="S44" s="42"/>
-      <c r="T44" s="42"/>
-      <c r="U44" s="42"/>
-      <c r="V44" s="42"/>
-      <c r="W44" s="42"/>
-    </row>
-    <row r="45" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E45" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J45" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K45" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L45" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M45" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N45" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O45" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P45" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q45" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R45" s="42"/>
-      <c r="S45" s="42"/>
-      <c r="T45" s="42"/>
-      <c r="U45" s="42"/>
-      <c r="V45" s="42"/>
-      <c r="W45" s="42"/>
-    </row>
-    <row r="46" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E46" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J46" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K46" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L46" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M46" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N46" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O46" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P46" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q46" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R46" s="42"/>
-      <c r="S46" s="42"/>
-      <c r="T46" s="42"/>
-      <c r="U46" s="42"/>
-      <c r="V46" s="42"/>
-      <c r="W46" s="42"/>
-    </row>
-    <row r="47" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E47" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="F47" s="42"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J47" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="K47" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="L47" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M47" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="N47" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="O47" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P47" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q47" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="R47" s="42"/>
-      <c r="S47" s="45"/>
-      <c r="T47" s="42"/>
-      <c r="U47" s="42"/>
-      <c r="V47" s="45"/>
-      <c r="W47" s="42"/>
-    </row>
-    <row r="48" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E48" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" s="42"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J48" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="K48" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="L48" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M48" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="N48" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="O48" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P48" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q48" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="R48" s="42"/>
-      <c r="S48" s="45"/>
-      <c r="T48" s="42"/>
-      <c r="U48" s="42"/>
-      <c r="V48" s="45"/>
-      <c r="W48" s="42"/>
-    </row>
-    <row r="49" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E49" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="F49" s="43"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="J49" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="K49" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="L49" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="M49" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="N49" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="O49" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="P49" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q49" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="R49" s="43"/>
-      <c r="S49" s="45"/>
-      <c r="T49" s="42"/>
-      <c r="U49" s="43"/>
-      <c r="V49" s="45"/>
-      <c r="W49" s="42"/>
-    </row>
-    <row r="50" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E50" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J50" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K50" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L50" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M50" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N50" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O50" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P50" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q50" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R50" s="42"/>
-      <c r="S50" s="42"/>
-      <c r="T50" s="42"/>
-      <c r="U50" s="42"/>
-      <c r="V50" s="42"/>
-      <c r="W50" s="42"/>
-    </row>
-    <row r="51" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E51" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J51" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="K51" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L51" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="M51" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="N51" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="O51" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P51" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q51" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R51" s="42"/>
-      <c r="S51" s="42"/>
-      <c r="T51" s="42"/>
-      <c r="U51" s="42"/>
-      <c r="V51" s="42"/>
-      <c r="W51" s="42"/>
+      <c r="H68" s="42" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="O11:Q11"/>
     <mergeCell ref="U40:W40"/>
     <mergeCell ref="E40:E42"/>
     <mergeCell ref="F40:H40"/>
@@ -2650,17 +2975,17 @@
     <mergeCell ref="L40:N40"/>
     <mergeCell ref="O40:Q40"/>
     <mergeCell ref="R40:T40"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:N26"/>
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2669,22 +2994,22 @@
   <dimension ref="D5:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36:I37"/>
+      <selection activeCell="K33" sqref="K33:L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="6.33203125" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="4:10" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="4:10" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="9" t="s">
         <v>0</v>
       </c>
@@ -2701,13 +3026,13 @@
         <v>4</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="12">
         <v>2017</v>
       </c>
@@ -2730,7 +3055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3">
         <v>2017</v>
       </c>
@@ -2753,7 +3078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="14">
         <v>2017</v>
       </c>
@@ -2773,10 +3098,10 @@
         <v>23</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="15">
         <v>2018</v>
       </c>
@@ -2799,7 +3124,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D11" s="4">
         <v>2018</v>
       </c>
@@ -2819,10 +3144,10 @@
         <v>23</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="16">
         <v>2018</v>
       </c>
@@ -2836,14 +3161,14 @@
         <v>22</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="I12" s="26"/>
       <c r="J12" s="27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="18">
         <v>2019</v>
       </c>
@@ -2863,10 +3188,10 @@
         <v>23</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="5">
         <v>2019</v>
       </c>
@@ -2886,10 +3211,10 @@
         <v>23</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="5">
         <v>2019</v>
       </c>
@@ -2903,16 +3228,16 @@
         <v>22</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="5">
         <v>2019</v>
       </c>
@@ -2926,16 +3251,16 @@
         <v>22</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="5">
         <v>2019</v>
       </c>
@@ -2949,16 +3274,16 @@
         <v>22</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="19">
         <v>2019</v>
       </c>
@@ -2971,8 +3296,8 @@
       <c r="G18" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="25" t="s">
-        <v>24</v>
+      <c r="H18" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>23</v>
@@ -2981,36 +3306,36 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="17">
         <v>2020</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J19" s="29"/>
     </row>
-    <row r="20" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="6">
         <v>2020</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>22</v>
@@ -3019,166 +3344,166 @@
         <v>23</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J20" s="24"/>
     </row>
-    <row r="21" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="6">
         <v>2020</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J21" s="24"/>
     </row>
-    <row r="22" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="6">
         <v>2020</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J22" s="24"/>
     </row>
-    <row r="23" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="6">
         <v>2020</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J23" s="24"/>
     </row>
-    <row r="24" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="6">
         <v>2020</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J24" s="24"/>
     </row>
-    <row r="25" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="6">
         <v>2020</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G25" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J25" s="24"/>
     </row>
-    <row r="26" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="6">
         <v>2020</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J26" s="24"/>
     </row>
-    <row r="27" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="6">
         <v>2020</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J27" s="24"/>
     </row>
-    <row r="28" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="6">
         <v>2020</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G28" s="25" t="s">
         <v>22</v>
@@ -3187,82 +3512,82 @@
         <v>23</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J28" s="24"/>
     </row>
-    <row r="29" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="6">
         <v>2020</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G29" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H29" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J29" s="24"/>
     </row>
-    <row r="30" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="6">
         <v>2020</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G30" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J30" s="32"/>
     </row>
-    <row r="31" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="6">
         <v>2020</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J31" s="32"/>
     </row>
-    <row r="32" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="6">
         <v>2020</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G32" s="25" t="s">
         <v>22</v>
@@ -3271,19 +3596,19 @@
         <v>23</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J32" s="32"/>
     </row>
-    <row r="33" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="6">
         <v>2020</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G33" s="25" t="s">
         <v>22</v>
@@ -3292,19 +3617,19 @@
         <v>23</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J33" s="32"/>
     </row>
-    <row r="34" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="6">
         <v>2020</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G34" s="25" t="s">
         <v>22</v>
@@ -3313,19 +3638,19 @@
         <v>23</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J34" s="32"/>
     </row>
-    <row r="35" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="6">
         <v>2020</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G35" s="25" t="s">
         <v>22</v>
@@ -3334,19 +3659,19 @@
         <v>23</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J35" s="32"/>
     </row>
-    <row r="36" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="6">
         <v>2020</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G36" s="25" t="s">
         <v>22</v>
@@ -3359,15 +3684,15 @@
       </c>
       <c r="J36" s="32"/>
     </row>
-    <row r="37" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="6">
         <v>2020</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G37" s="25" t="s">
         <v>22</v>
@@ -3380,15 +3705,15 @@
       </c>
       <c r="J37" s="32"/>
     </row>
-    <row r="38" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="6">
         <v>2020</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G38" s="25" t="s">
         <v>22</v>
@@ -3397,15 +3722,15 @@
       <c r="I38" s="31"/>
       <c r="J38" s="32"/>
     </row>
-    <row r="39" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="7">
         <v>2020</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F39" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G39" s="25" t="s">
         <v>22</v>

</xml_diff>